<commit_message>
db restructure – added conditional seeding in table models
</commit_message>
<xml_diff>
--- a/docs/db_schema_plan.xlsx
+++ b/docs/db_schema_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamstephan/Documents/GitHub/sharemyski/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{454AD7D5-DABF-324D-8A5F-ACA338B99141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABDEFB2-146D-D74D-BA8D-36FDAC92A8FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="5200" windowWidth="28040" windowHeight="17440" xr2:uid="{05E2CCC2-50E1-9A45-A769-233521CF17F5}"/>
+    <workbookView xWindow="16640" yWindow="10600" windowWidth="28040" windowHeight="17440" xr2:uid="{05E2CCC2-50E1-9A45-A769-233521CF17F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="79">
   <si>
     <t>User</t>
   </si>
@@ -41,174 +41,42 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>user_renter</t>
-  </si>
-  <si>
-    <t>user_rentor</t>
-  </si>
-  <si>
-    <t>user_home</t>
-  </si>
-  <si>
     <t>location</t>
   </si>
   <si>
     <t>loc_id</t>
   </si>
   <si>
-    <t>loc_address1</t>
-  </si>
-  <si>
-    <t>loc_address2</t>
-  </si>
-  <si>
-    <t>loc_city</t>
-  </si>
-  <si>
-    <t>loc_state</t>
-  </si>
-  <si>
-    <t>loc_country</t>
-  </si>
-  <si>
     <t>bool</t>
   </si>
   <si>
     <t>int</t>
   </si>
   <si>
-    <t>char</t>
-  </si>
-  <si>
     <t xml:space="preserve">? </t>
   </si>
   <si>
-    <t>gear</t>
-  </si>
-  <si>
-    <t>user_name</t>
-  </si>
-  <si>
-    <t>user_phone</t>
-  </si>
-  <si>
-    <t>gear_id</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
     <t>cat_id</t>
   </si>
   <si>
-    <t>cat_name</t>
-  </si>
-  <si>
-    <t>loc_lon</t>
-  </si>
-  <si>
     <t xml:space="preserve">int </t>
   </si>
   <si>
-    <t>loc_lat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">char  </t>
-  </si>
-  <si>
-    <t>char/u</t>
-  </si>
-  <si>
     <t>int/inc/u</t>
   </si>
   <si>
-    <t>user_renter_rating</t>
-  </si>
-  <si>
-    <t>user_rentor_rating</t>
-  </si>
-  <si>
-    <t>gear_rating</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
-    <t>gear_desc</t>
-  </si>
-  <si>
-    <t>gear_gender</t>
-  </si>
-  <si>
-    <t>tranactions</t>
-  </si>
-  <si>
-    <t>tran_id</t>
-  </si>
-  <si>
-    <t>tran_rentor</t>
-  </si>
-  <si>
-    <t>tran_renter</t>
-  </si>
-  <si>
-    <t>tran_start</t>
-  </si>
-  <si>
-    <t>tran_stop</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>tran_days</t>
-  </si>
-  <si>
-    <t>tran_total</t>
-  </si>
-  <si>
-    <t>gear_rate</t>
-  </si>
-  <si>
-    <t>tran_insurance</t>
-  </si>
-  <si>
     <t>m/w/u</t>
   </si>
   <si>
-    <t>user_auth_id</t>
-  </si>
-  <si>
-    <t>user_email</t>
-  </si>
-  <si>
-    <t>tran_rentor_rating</t>
-  </si>
-  <si>
-    <t>tran_daily_rate</t>
-  </si>
-  <si>
-    <t>tran_renter_rating</t>
-  </si>
-  <si>
-    <t>user_renter_total</t>
-  </si>
-  <si>
-    <t>user_rentor_total</t>
-  </si>
-  <si>
-    <t>user_renter_trans</t>
-  </si>
-  <si>
-    <t>user_rentor_trans</t>
-  </si>
-  <si>
-    <t>gear_image</t>
-  </si>
-  <si>
-    <t>char/url</t>
-  </si>
-  <si>
     <t>User table:</t>
   </si>
   <si>
@@ -230,34 +98,178 @@
     <t>trans to user = one to one (twice)</t>
   </si>
   <si>
-    <t>trans to gear = one to one</t>
-  </si>
-  <si>
     <t>Transaction table:</t>
   </si>
   <si>
-    <t>ref by: gear and trans tables</t>
-  </si>
-  <si>
-    <t>ref by user and gear tables</t>
-  </si>
-  <si>
     <t>ref by: trans table</t>
   </si>
   <si>
-    <t>ref by: gear table</t>
-  </si>
-  <si>
     <t>Category table:</t>
   </si>
   <si>
     <t>ref by: none</t>
   </si>
   <si>
-    <t>Gear table:</t>
-  </si>
-  <si>
     <t>Database Schema Design Plan</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>fb_id</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>rents</t>
+  </si>
+  <si>
+    <t>owns</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>renter_rating_avg</t>
+  </si>
+  <si>
+    <t>owner_rating_avg</t>
+  </si>
+  <si>
+    <t>renter_transactions</t>
+  </si>
+  <si>
+    <t>owner_transactions</t>
+  </si>
+  <si>
+    <t>renter_total_value</t>
+  </si>
+  <si>
+    <t>owner_total_value</t>
+  </si>
+  <si>
+    <t>ref by: stuff and transactions tables</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>address2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>string/u</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string  </t>
+  </si>
+  <si>
+    <t>string/url</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>transactions</t>
+  </si>
+  <si>
+    <t>ref by user and stuff tables</t>
+  </si>
+  <si>
+    <t>stuff</t>
+  </si>
+  <si>
+    <t>Stuff table:</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>renter</t>
+  </si>
+  <si>
+    <t>stuff_id</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>insurance</t>
+  </si>
+  <si>
+    <t>daily_rate</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>renter_rating</t>
+  </si>
+  <si>
+    <t>owner_rating</t>
+  </si>
+  <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>updatedAt</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>trans to stuff = one to one</t>
+  </si>
+  <si>
+    <t>ref by: stuff table</t>
   </si>
 </sst>
 </file>
@@ -640,12 +652,12 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="1.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -663,7 +675,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -686,66 +698,66 @@
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="H3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="K3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>1</v>
@@ -754,13 +766,13 @@
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>1</v>
@@ -768,27 +780,31 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="M6" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>1</v>
@@ -796,214 +812,238 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="M7" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="M9" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="M10" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="M11" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G12" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="M12" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="M13" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1012,18 +1052,18 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="M15" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1031,15 +1071,19 @@
       <c r="H16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1047,12 +1091,20 @@
       <c r="H17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="M17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="G18" s="1"/>
@@ -1063,8 +1115,12 @@
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="G19" s="1"/>
@@ -1075,8 +1131,12 @@
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="G20" s="1"/>
@@ -1087,8 +1147,12 @@
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="G21" s="1"/>
@@ -1100,73 +1164,73 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="J23" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="M23" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="J24" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="M24" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="M25" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G26" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="M26" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup scale="86" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="82" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>